<commit_message>
update to biosteam 2.14.4
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/cornstover/Spearman correlation cornstover.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/cornstover/Spearman correlation cornstover.xlsx
@@ -28,6 +28,147 @@
     <t>Saccharification and co fermentation-R301 ethanol conversion [0.93, 0.95, 0.97]</t>
   </si>
   <si>
+    <t>Seed hold tank pump base cost (USD) [7.38e+03, 8.2e+03, 9.02e+03]</t>
+  </si>
+  <si>
+    <t>Seed hold tank pump exponent [0.7, 0.8, 0.9]</t>
+  </si>
+  <si>
+    <t>Seed hold tank pump electricity rate (kW / kg/hr) [0.000156, 0.000173, 0.00019]</t>
+  </si>
+  <si>
+    <t>Seed hold tank tank base cost (USD) [3.95e+05, 4.39e+05, 4.83e+05]</t>
+  </si>
+  <si>
+    <t>Seed hold tank tank exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Seed hold tank agitator base cost (USD) [2.86e+04, 3.18e+04, 3.5e+04]</t>
+  </si>
+  <si>
+    <t>Seed hold tank agitator exponent [0.4, 0.5, 0.6]</t>
+  </si>
+  <si>
+    <t>Seed hold tank agitator electricity rate (kW / kg/hr) [0.000252, 0.00028, 0.000308]</t>
+  </si>
+  <si>
+    <t>Pretreatment flash tank base cost (USD) [4.6e+05, 5.11e+05, 5.62e+05]</t>
+  </si>
+  <si>
+    <t>Pretreatment flash tank exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Pretreatment flash pump base cost (USD) [2.7e+04, 3e+04, 3.3e+04]</t>
+  </si>
+  <si>
+    <t>Pretreatment flash pump exponent [0.7, 0.8, 0.9]</t>
+  </si>
+  <si>
+    <t>Pretreatment flash pump electricity rate (kW / kg/hr) [0.000199, 0.000221, 0.000243]</t>
+  </si>
+  <si>
+    <t>Pretreatment flash agitator base cost (USD) [8.1e+04, 9e+04, 9.9e+04]</t>
+  </si>
+  <si>
+    <t>Pretreatment flash agitator exponent [0.4, 0.5, 0.6]</t>
+  </si>
+  <si>
+    <t>Pretreatment flash agitator electricity rate (kW / kg/hr) [0.000605, 0.000672, 0.000739]</t>
+  </si>
+  <si>
+    <t>Fire water tank bag base cost (USD) [2.7e+04, 3e+04, 3.3e+04]</t>
+  </si>
+  <si>
+    <t>Fire water tank bag exponent [0.5, 0.6, 0.7]</t>
+  </si>
+  <si>
+    <t>Fire water tank tank base cost (USD) [7.23e+05, 8.03e+05, 8.83e+05]</t>
+  </si>
+  <si>
+    <t>Fire water tank tank exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Fire water tank pump base cost (USD) [1.35e+04, 1.5e+04, 1.65e+04]</t>
+  </si>
+  <si>
+    <t>Fire water tank pump exponent [0.7, 0.8, 0.9]</t>
+  </si>
+  <si>
+    <t>Fire water tank pump electricity rate (kW / kg/hr) [0.0102, 0.0113, 0.0124]</t>
+  </si>
+  <si>
+    <t>Waste water system cost waste water system base cost (USD) [4.53e+07, 5.03e+07, 5.53e+07]</t>
+  </si>
+  <si>
+    <t>Waste water system cost waste water system exponent [0.5, 0.6, 0.7]</t>
+  </si>
+  <si>
+    <t>Waste water system cost waste water system electricity rate (kW / kg/hr) [0.0156, 0.0173, 0.019]</t>
+  </si>
+  <si>
+    <t>Feed stock handling system exponent [0.5, 0.6, 0.7]</t>
+  </si>
+  <si>
+    <t>Feed stock handling system electricity rate (kW / kg/hr) [0.00744, 0.00827, 0.0091]</t>
+  </si>
+  <si>
+    <t>Seed train stage #5 agitators base cost (USD) [1.94e+04, 2.15e+04, 2.37e+04]</t>
+  </si>
+  <si>
+    <t>Seed train stage #5 agitators exponent [0.4, 0.5, 0.6]</t>
+  </si>
+  <si>
+    <t>Seed train stage #5 agitators electricity rate (kW / m3) [0.0119, 0.0132, 0.0145]</t>
+  </si>
+  <si>
+    <t>Seed train stage #5 reactors base cost (USD) [5.31e+05, 5.9e+05, 6.49e+05]</t>
+  </si>
+  <si>
+    <t>Seed train stage #5 reactors exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Seed train stage #4 agitators base cost (USD) [1.17e+04, 1.3e+04, 1.43e+04]</t>
+  </si>
+  <si>
+    <t>Seed train stage #4 agitators exponent [0.4, 0.5, 0.6]</t>
+  </si>
+  <si>
+    <t>Seed train stage #4 agitators electricity rate (kW / m3) [0.0892, 0.0991, 0.109]</t>
+  </si>
+  <si>
+    <t>Seed train stage #4 reactors base cost (USD) [1.58e+05, 1.76e+05, 1.94e+05]</t>
+  </si>
+  <si>
+    <t>Seed train stage #4 reactors exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Seed train stage #3 reactors base cost (USD) [7.09e+04, 7.88e+04, 8.67e+04]</t>
+  </si>
+  <si>
+    <t>Seed train stage #3 reactors exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Seed train stage #2 reactors base cost (USD) [5.25e+04, 5.83e+04, 6.41e+04]</t>
+  </si>
+  <si>
+    <t>Seed train stage #2 reactors exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Seed train stage #1 reactors base cost (USD) [3.39e+04, 3.77e+04, 4.15e+04]</t>
+  </si>
+  <si>
+    <t>Seed train stage #1 reactors exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Seed train pumps base cost (USD) [2.23e+04, 2.48e+04, 2.73e+04]</t>
+  </si>
+  <si>
+    <t>Seed train pumps exponent [0.7, 0.8, 0.9]</t>
+  </si>
+  <si>
+    <t>Seed train pumps electricity rate (kW / kg/hr) [0.000834, 0.000927, 0.00102]</t>
+  </si>
+  <si>
     <t>Molecular sieve column base cost (USD) [2.34e+06, 2.6e+06, 2.86e+06]</t>
   </si>
   <si>
@@ -37,6 +178,36 @@
     <t>Molecular sieve column electricity rate (kW / kg/hr) [0.00599, 0.00666, 0.00732]</t>
   </si>
   <si>
+    <t>DAPTank tank base cost (USD) [9.18e+04, 1.02e+05, 1.12e+05]</t>
+  </si>
+  <si>
+    <t>DAPTank tank exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>DAPTank pump base cost (USD) [2.7e+03, 3e+03, 3.3e+03]</t>
+  </si>
+  <si>
+    <t>DAPTank pump exponent [0.7, 0.8, 0.9]</t>
+  </si>
+  <si>
+    <t>DAPTank pump electricity rate (kW / kg/hr) [0.00208, 0.00232, 0.00255]</t>
+  </si>
+  <si>
+    <t>DAPTank agitator base cost (USD) [8.82e+03, 9.8e+03, 1.08e+04]</t>
+  </si>
+  <si>
+    <t>DAPTank agitator exponent [0.4, 0.5, 0.6]</t>
+  </si>
+  <si>
+    <t>DAPTank agitator electricity rate (kW / kg/hr) [0.0226, 0.0252, 0.0277]</t>
+  </si>
+  <si>
+    <t>Waste vapor condenser heat exchanger base cost (USD) [3.06e+04, 3.4e+04, 3.74e+04]</t>
+  </si>
+  <si>
+    <t>Waste vapor condenser heat exchanger exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
     <t>Air distribution package plant air compressor base cost (USD) [2.52e+04, 2.8e+04, 3.08e+04]</t>
   </si>
   <si>
@@ -58,102 +229,36 @@
     <t>Air distribution package plant air reciever exponent [0.5, 0.6, 0.7]</t>
   </si>
   <si>
-    <t>Waste water system cost waste water system base cost (USD) [4.53e+07, 5.03e+07, 5.53e+07]</t>
-  </si>
-  <si>
-    <t>Waste water system cost waste water system exponent [0.5, 0.6, 0.7]</t>
-  </si>
-  <si>
-    <t>Waste water system cost waste water system electricity rate (kW / kg/hr) [0.0156, 0.0173, 0.019]</t>
-  </si>
-  <si>
-    <t>DAPTank tank base cost (USD) [9.18e+04, 1.02e+05, 1.12e+05]</t>
-  </si>
-  <si>
-    <t>DAPTank tank exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>DAPTank pump base cost (USD) [2.7e+03, 3e+03, 3.3e+03]</t>
-  </si>
-  <si>
-    <t>DAPTank pump exponent [0.7, 0.8, 0.9]</t>
-  </si>
-  <si>
-    <t>DAPTank pump electricity rate (kW / kg/hr) [0.00208, 0.00232, 0.00255]</t>
-  </si>
-  <si>
-    <t>DAPTank agitator base cost (USD) [8.82e+03, 9.8e+03, 1.08e+04]</t>
-  </si>
-  <si>
-    <t>DAPTank agitator exponent [0.4, 0.5, 0.6]</t>
-  </si>
-  <si>
-    <t>DAPTank agitator electricity rate (kW / kg/hr) [0.0226, 0.0252, 0.0277]</t>
-  </si>
-  <si>
-    <t>Seed hold tank pump base cost (USD) [7.38e+03, 8.2e+03, 9.02e+03]</t>
-  </si>
-  <si>
-    <t>Seed hold tank pump exponent [0.7, 0.8, 0.9]</t>
-  </si>
-  <si>
-    <t>Seed hold tank pump electricity rate (kW / kg/hr) [0.000156, 0.000173, 0.00019]</t>
-  </si>
-  <si>
-    <t>Seed hold tank tank base cost (USD) [3.95e+05, 4.39e+05, 4.83e+05]</t>
-  </si>
-  <si>
-    <t>Seed hold tank tank exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Seed hold tank agitator base cost (USD) [2.86e+04, 3.18e+04, 3.5e+04]</t>
-  </si>
-  <si>
-    <t>Seed hold tank agitator exponent [0.4, 0.5, 0.6]</t>
-  </si>
-  <si>
-    <t>Seed hold tank agitator electricity rate (kW / kg/hr) [0.000252, 0.00028, 0.000308]</t>
-  </si>
-  <si>
-    <t>Feed stock handling system exponent [0.5, 0.6, 0.7]</t>
-  </si>
-  <si>
-    <t>Feed stock handling system electricity rate (kW / kg/hr) [0.00744, 0.00827, 0.0091]</t>
-  </si>
-  <si>
-    <t>Waste vapor condenser heat exchanger base cost (USD) [3.06e+04, 3.4e+04, 3.74e+04]</t>
-  </si>
-  <si>
-    <t>Waste vapor condenser heat exchanger exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Fire water tank bag base cost (USD) [2.7e+04, 3e+04, 3.3e+04]</t>
-  </si>
-  <si>
-    <t>Fire water tank bag exponent [0.5, 0.6, 0.7]</t>
-  </si>
-  <si>
-    <t>Fire water tank tank base cost (USD) [7.23e+05, 8.03e+05, 8.83e+05]</t>
-  </si>
-  <si>
-    <t>Fire water tank tank exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Fire water tank pump base cost (USD) [1.35e+04, 1.5e+04, 1.65e+04]</t>
-  </si>
-  <si>
-    <t>Fire water tank pump exponent [0.7, 0.8, 0.9]</t>
-  </si>
-  <si>
-    <t>Fire water tank pump electricity rate (kW / kg/hr) [0.0102, 0.0113, 0.0124]</t>
-  </si>
-  <si>
     <t>Ammonia mixer mixer base cost (USD) [4.5e+03, 5e+03, 5.5e+03]</t>
   </si>
   <si>
     <t>Ammonia mixer mixer exponent [0.4, 0.5, 0.6]</t>
   </si>
   <si>
+    <t>Process water center tank base cost (USD) [2.25e+05, 2.5e+05, 2.75e+05]</t>
+  </si>
+  <si>
+    <t>Process water center tank exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Process water center process water pump base cost (USD) [1.38e+04, 1.53e+04, 1.68e+04]</t>
+  </si>
+  <si>
+    <t>Process water center process water pump exponent [0.7, 0.8, 0.9]</t>
+  </si>
+  <si>
+    <t>Process water center process water pump electricity rate (kW / kg/hr) [9.7e-05, 0.000108, 0.000119]</t>
+  </si>
+  <si>
+    <t>Process water center makeup water pump base cost (USD) [6.18e+03, 6.86e+03, 7.55e+03]</t>
+  </si>
+  <si>
+    <t>Process water center makeup water pump exponent [0.7, 0.8, 0.9]</t>
+  </si>
+  <si>
+    <t>Process water center makeup water pump electricity rate (kW / kg/hr) [8.63e-05, 9.59e-05, 0.000105]</t>
+  </si>
+  <si>
     <t>CSLTank tank base cost (USD) [6.3e+04, 7e+04, 7.7e+04]</t>
   </si>
   <si>
@@ -178,61 +283,211 @@
     <t>CSLTank agitator electricity rate (kW / kg/hr) [0.00482, 0.00535, 0.00589]</t>
   </si>
   <si>
-    <t>Seed train stage #5 agitators base cost (USD) [1.94e+04, 2.15e+04, 2.37e+04]</t>
-  </si>
-  <si>
-    <t>Seed train stage #5 agitators exponent [0.4, 0.5, 0.6]</t>
-  </si>
-  <si>
-    <t>Seed train stage #5 agitators electricity rate (kW / m3) [0.0119, 0.0132, 0.0145]</t>
-  </si>
-  <si>
-    <t>Seed train stage #5 reactors base cost (USD) [5.31e+05, 5.9e+05, 6.49e+05]</t>
-  </si>
-  <si>
-    <t>Seed train stage #5 reactors exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Seed train stage #4 agitators base cost (USD) [1.17e+04, 1.3e+04, 1.43e+04]</t>
-  </si>
-  <si>
-    <t>Seed train stage #4 agitators exponent [0.4, 0.5, 0.6]</t>
-  </si>
-  <si>
-    <t>Seed train stage #4 agitators electricity rate (kW / m3) [0.0892, 0.0991, 0.109]</t>
-  </si>
-  <si>
-    <t>Seed train stage #4 reactors base cost (USD) [1.58e+05, 1.76e+05, 1.94e+05]</t>
-  </si>
-  <si>
-    <t>Seed train stage #4 reactors exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Seed train stage #3 reactors base cost (USD) [7.09e+04, 7.88e+04, 8.67e+04]</t>
-  </si>
-  <si>
-    <t>Seed train stage #3 reactors exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Seed train stage #2 reactors base cost (USD) [5.25e+04, 5.83e+04, 6.41e+04]</t>
-  </si>
-  <si>
-    <t>Seed train stage #2 reactors exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Seed train stage #1 reactors base cost (USD) [3.39e+04, 3.77e+04, 4.15e+04]</t>
-  </si>
-  <si>
-    <t>Seed train stage #1 reactors exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Seed train pumps base cost (USD) [2.23e+04, 2.48e+04, 2.73e+04]</t>
-  </si>
-  <si>
-    <t>Seed train pumps exponent [0.7, 0.8, 0.9]</t>
-  </si>
-  <si>
-    <t>Seed train pumps electricity rate (kW / kg/hr) [0.000834, 0.000927, 0.00102]</t>
+    <t>Pretreatment reactor system base cost (USD) [1.78e+07, 1.98e+07, 2.18e+07]</t>
+  </si>
+  <si>
+    <t>Pretreatment reactor system exponent [0.5, 0.6, 0.7]</t>
+  </si>
+  <si>
+    <t>Pretreatment reactor system electricity rate (kW / kg/hr) [0.0494, 0.0549, 0.0604]</t>
+  </si>
+  <si>
+    <t>Ammonia addition tank tank base cost (USD) [2.12e+05, 2.36e+05, 2.6e+05]</t>
+  </si>
+  <si>
+    <t>Ammonia addition tank tank exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Ammonia addition tank agitator base cost (USD) [1.97e+04, 2.19e+04, 2.41e+04]</t>
+  </si>
+  <si>
+    <t>Ammonia addition tank agitator exponent [0.4, 0.5, 0.6]</t>
+  </si>
+  <si>
+    <t>Ammonia addition tank agitator electricity rate (kW / kg/hr) [1.64e-05, 1.82e-05, 2e-05]</t>
+  </si>
+  <si>
+    <t>Hydrolysate cooler heat exchanger base cost (USD) [7.65e+04, 8.5e+04, 9.35e+04]</t>
+  </si>
+  <si>
+    <t>Hydrolysate cooler heat exchanger exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Pressure filter dry air pressure filter (2) base cost (USD) [3.64e+05, 4.05e+05, 4.46e+05]</t>
+  </si>
+  <si>
+    <t>Pressure filter dry air pressure filter (2) exponent [0.5, 0.6, 0.7]</t>
+  </si>
+  <si>
+    <t>Pressure filter dry air pressure filter (2) electricity rate (kW / kg/hr) [0.0295, 0.0328, 0.0361]</t>
+  </si>
+  <si>
+    <t>Pressure filter pressing air pressure filter base cost (USD) [6.77e+04, 7.52e+04, 8.27e+04]</t>
+  </si>
+  <si>
+    <t>Pressure filter pressing air pressure filter exponent [0.5, 0.6, 0.7]</t>
+  </si>
+  <si>
+    <t>Pressure filter pressing air pressure filter electricity rate (kW / kg/hr) [0.00317, 0.00352, 0.00387]</t>
+  </si>
+  <si>
+    <t>Pressure filter dry air compressor receiver tank base cost (USD) [1.53e+04, 1.7e+04, 1.87e+04]</t>
+  </si>
+  <si>
+    <t>Pressure filter dry air compressor receiver tank exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Pressure filter cloth wash pump base cost (USD) [2.62e+04, 2.92e+04, 3.21e+04]</t>
+  </si>
+  <si>
+    <t>Pressure filter cloth wash pump exponent [0.7, 0.8, 0.9]</t>
+  </si>
+  <si>
+    <t>Pressure filter cloth wash pump electricity rate (kW / kg/hr) [0.00316, 0.00352, 0.00387]</t>
+  </si>
+  <si>
+    <t>Pressure filter pressing air compressor receiver tank base cost (USD) [7.2e+03, 8e+03, 8.8e+03]</t>
+  </si>
+  <si>
+    <t>Pressure filter pressing air compressor receiver tank exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Pressure filter base cost (USD) [2.97e+06, 3.29e+06, 3.62e+06]</t>
+  </si>
+  <si>
+    <t>Pressure filter exponent [0.7, 0.8, 0.9]</t>
+  </si>
+  <si>
+    <t>Pressure filter lignin wet cake conveyor base cost (USD) [6.3e+04, 7e+04, 7.7e+04]</t>
+  </si>
+  <si>
+    <t>Pressure filter lignin wet cake conveyor exponent [0.7, 0.8, 0.9]</t>
+  </si>
+  <si>
+    <t>Pressure filter lignin wet cake conveyor electricity rate (kW / kg/hr) [0.000234, 0.00026, 0.000287]</t>
+  </si>
+  <si>
+    <t>Pressure filter lignin wet cake screw base cost (USD) [1.8e+04, 2e+04, 2.2e+04]</t>
+  </si>
+  <si>
+    <t>Pressure filter lignin wet cake screw exponent [0.7, 0.8, 0.9]</t>
+  </si>
+  <si>
+    <t>Pressure filter lignin wet cake screw electricity rate (kW / kg/hr) [0.000352, 0.000391, 0.00043]</t>
+  </si>
+  <si>
+    <t>Pressure filter recycled water tank base cost (USD) [1.37e+03, 1.52e+03, 1.67e+03]</t>
+  </si>
+  <si>
+    <t>Pressure filter recycled water tank exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Pressure filter mafifold flush pump base cost (USD) [1.54e+04, 1.71e+04, 1.88e+04]</t>
+  </si>
+  <si>
+    <t>Pressure filter mafifold flush pump exponent [0.7, 0.8, 0.9]</t>
+  </si>
+  <si>
+    <t>Pressure filter mafifold flush pump electricity rate (kW / kg/hr) [0.00211, 0.00234, 0.00258]</t>
+  </si>
+  <si>
+    <t>Pressure filter stillage tank 531 base cost (USD) [1.57e+05, 1.75e+05, 1.92e+05]</t>
+  </si>
+  <si>
+    <t>Pressure filter stillage tank 531 exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Pressure filter feed pump base cost (USD) [1.64e+04, 1.82e+04, 2e+04]</t>
+  </si>
+  <si>
+    <t>Pressure filter feed pump exponent [0.7, 0.8, 0.9]</t>
+  </si>
+  <si>
+    <t>Pressure filter feed pump electricity rate (kW / kg/hr) [0.00211, 0.00234, 0.00258]</t>
+  </si>
+  <si>
+    <t>Pressure filter filtrate tank base cost (USD) [9.27e+04, 1.03e+05, 1.13e+05]</t>
+  </si>
+  <si>
+    <t>Pressure filter filtrate tank exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Pressure filter discharge pump base cost (USD) [1.17e+04, 1.3e+04, 1.43e+04]</t>
+  </si>
+  <si>
+    <t>Pressure filter discharge pump exponent [0.7, 0.8, 0.9]</t>
+  </si>
+  <si>
+    <t>Pressure filter flitrate tank agitator base cost (USD) [2.34e+04, 2.6e+04, 2.86e+04]</t>
+  </si>
+  <si>
+    <t>Pressure filter flitrate tank agitator exponent [0.4, 0.5, 0.6]</t>
+  </si>
+  <si>
+    <t>Pressure filter flitrate tank agitator electricity rate (kW / kg/hr) [0.000158, 0.000176, 0.000193]</t>
+  </si>
+  <si>
+    <t>Vent scrubber base cost (USD) [1.94e+05, 2.15e+05, 2.37e+05]</t>
+  </si>
+  <si>
+    <t>Vent scrubber exponent [0.5, 0.6, 0.7]</t>
+  </si>
+  <si>
+    <t>Boiler turbogenerator boiler base cost (USD) [2.57e+07, 2.86e+07, 3.14e+07]</t>
+  </si>
+  <si>
+    <t>Boiler turbogenerator boiler exponent [0.5, 0.6, 0.7]</t>
+  </si>
+  <si>
+    <t>Boiler turbogenerator boiler electricity rate (kW / kg/hr) [0.00377, 0.00419, 0.00461]</t>
+  </si>
+  <si>
+    <t>Boiler turbogenerator deaerator base cost (USD) [2.74e+05, 3.05e+05, 3.36e+05]</t>
+  </si>
+  <si>
+    <t>Boiler turbogenerator deaerator exponent [0.5, 0.6, 0.7]</t>
+  </si>
+  <si>
+    <t>Boiler turbogenerator amine addition pkg base cost (USD) [3.6e+04, 4e+04, 4.4e+04]</t>
+  </si>
+  <si>
+    <t>Boiler turbogenerator amine addition pkg exponent [0.5, 0.6, 0.7]</t>
+  </si>
+  <si>
+    <t>Boiler turbogenerator hot process water softener system base cost (USD) [7.02e+04, 7.8e+04, 8.58e+04]</t>
+  </si>
+  <si>
+    <t>Boiler turbogenerator hot process water softener system exponent [0.5, 0.6, 0.7]</t>
+  </si>
+  <si>
+    <t>Boiler turbogenerator turbogenerator base cost (USD) [8.55e+06, 9.5e+06, 1.04e+07]</t>
+  </si>
+  <si>
+    <t>Boiler turbogenerator turbogenerator exponent [0.5, 0.6, 0.7]</t>
+  </si>
+  <si>
+    <t>Enzyme hydrolysate mixer mixer base cost (USD) [9.81e+04, 1.09e+05, 1.2e+05]</t>
+  </si>
+  <si>
+    <t>Enzyme hydrolysate mixer mixer exponent [0.4, 0.5, 0.6]</t>
+  </si>
+  <si>
+    <t>Enzyme hydrolysate mixer mixer electricity rate (kW / kg/hr) [0.000177, 0.000196, 0.000216]</t>
+  </si>
+  <si>
+    <t>Sulfuric acid tank tank base cost (USD) [5.59e+03, 6.21e+03, 6.83e+03]</t>
+  </si>
+  <si>
+    <t>Sulfuric acid tank tank exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Sulfuric acid tank pump base cost (USD) [7.2e+03, 8e+03, 8.8e+03]</t>
+  </si>
+  <si>
+    <t>Sulfuric acid tank pump exponent [0.7, 0.8, 0.9]</t>
+  </si>
+  <si>
+    <t>Sulfuric acid tank pump electricity rate (kW / kg/hr) [0.000242, 0.000269, 0.000296]</t>
   </si>
   <si>
     <t>Sulfuric acid mixer mixer base cost (USD) [5.4e+03, 6e+03, 6.6e+03]</t>
@@ -241,220 +496,61 @@
     <t>Sulfuric acid mixer mixer exponent [0.4, 0.5, 0.6]</t>
   </si>
   <si>
-    <t>Ammonia addition tank tank base cost (USD) [2.12e+05, 2.36e+05, 2.6e+05]</t>
-  </si>
-  <si>
-    <t>Ammonia addition tank tank exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Ammonia addition tank agitator base cost (USD) [1.97e+04, 2.19e+04, 2.41e+04]</t>
-  </si>
-  <si>
-    <t>Ammonia addition tank agitator exponent [0.4, 0.5, 0.6]</t>
-  </si>
-  <si>
-    <t>Ammonia addition tank agitator electricity rate (kW / kg/hr) [1.64e-05, 1.82e-05, 2e-05]</t>
-  </si>
-  <si>
-    <t>Pressure filter dry air pressure filter (2) base cost (USD) [3.64e+05, 4.05e+05, 4.46e+05]</t>
-  </si>
-  <si>
-    <t>Pressure filter dry air pressure filter (2) exponent [0.5, 0.6, 0.7]</t>
-  </si>
-  <si>
-    <t>Pressure filter dry air pressure filter (2) electricity rate (kW / kg/hr) [0.0295, 0.0328, 0.0361]</t>
-  </si>
-  <si>
-    <t>Pressure filter pressing air pressure filter base cost (USD) [6.77e+04, 7.52e+04, 8.27e+04]</t>
-  </si>
-  <si>
-    <t>Pressure filter pressing air pressure filter exponent [0.5, 0.6, 0.7]</t>
-  </si>
-  <si>
-    <t>Pressure filter pressing air pressure filter electricity rate (kW / kg/hr) [0.00317, 0.00352, 0.00387]</t>
-  </si>
-  <si>
-    <t>Pressure filter dry air compressor receiver tank base cost (USD) [1.53e+04, 1.7e+04, 1.87e+04]</t>
-  </si>
-  <si>
-    <t>Pressure filter dry air compressor receiver tank exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Pressure filter cloth wash pump base cost (USD) [2.62e+04, 2.92e+04, 3.21e+04]</t>
-  </si>
-  <si>
-    <t>Pressure filter cloth wash pump exponent [0.7, 0.8, 0.9]</t>
-  </si>
-  <si>
-    <t>Pressure filter cloth wash pump electricity rate (kW / kg/hr) [0.00316, 0.00352, 0.00387]</t>
-  </si>
-  <si>
-    <t>Pressure filter pressing air compressor receiver tank base cost (USD) [7.2e+03, 8e+03, 8.8e+03]</t>
-  </si>
-  <si>
-    <t>Pressure filter pressing air compressor receiver tank exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Pressure filter base cost (USD) [2.97e+06, 3.29e+06, 3.62e+06]</t>
-  </si>
-  <si>
-    <t>Pressure filter exponent [0.7, 0.8, 0.9]</t>
-  </si>
-  <si>
-    <t>Pressure filter lignin wet cake conveyor base cost (USD) [6.3e+04, 7e+04, 7.7e+04]</t>
-  </si>
-  <si>
-    <t>Pressure filter lignin wet cake conveyor exponent [0.7, 0.8, 0.9]</t>
-  </si>
-  <si>
-    <t>Pressure filter lignin wet cake conveyor electricity rate (kW / kg/hr) [0.000234, 0.00026, 0.000287]</t>
-  </si>
-  <si>
-    <t>Pressure filter lignin wet cake screw base cost (USD) [1.8e+04, 2e+04, 2.2e+04]</t>
-  </si>
-  <si>
-    <t>Pressure filter lignin wet cake screw exponent [0.7, 0.8, 0.9]</t>
-  </si>
-  <si>
-    <t>Pressure filter lignin wet cake screw electricity rate (kW / kg/hr) [0.000352, 0.000391, 0.00043]</t>
-  </si>
-  <si>
-    <t>Pressure filter recycled water tank base cost (USD) [1.37e+03, 1.52e+03, 1.67e+03]</t>
-  </si>
-  <si>
-    <t>Pressure filter recycled water tank exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Pressure filter mafifold flush pump base cost (USD) [1.54e+04, 1.71e+04, 1.88e+04]</t>
-  </si>
-  <si>
-    <t>Pressure filter mafifold flush pump exponent [0.7, 0.8, 0.9]</t>
-  </si>
-  <si>
-    <t>Pressure filter mafifold flush pump electricity rate (kW / kg/hr) [0.00211, 0.00234, 0.00258]</t>
-  </si>
-  <si>
-    <t>Pressure filter stillage tank 531 base cost (USD) [1.57e+05, 1.75e+05, 1.92e+05]</t>
-  </si>
-  <si>
-    <t>Pressure filter stillage tank 531 exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Pressure filter feed pump base cost (USD) [1.64e+04, 1.82e+04, 2e+04]</t>
-  </si>
-  <si>
-    <t>Pressure filter feed pump exponent [0.7, 0.8, 0.9]</t>
-  </si>
-  <si>
-    <t>Pressure filter feed pump electricity rate (kW / kg/hr) [0.00211, 0.00234, 0.00258]</t>
-  </si>
-  <si>
-    <t>Pressure filter filtrate tank base cost (USD) [9.27e+04, 1.03e+05, 1.13e+05]</t>
-  </si>
-  <si>
-    <t>Pressure filter filtrate tank exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Pressure filter discharge pump base cost (USD) [1.17e+04, 1.3e+04, 1.43e+04]</t>
-  </si>
-  <si>
-    <t>Pressure filter discharge pump exponent [0.7, 0.8, 0.9]</t>
-  </si>
-  <si>
-    <t>Pressure filter flitrate tank agitator base cost (USD) [2.34e+04, 2.6e+04, 2.86e+04]</t>
-  </si>
-  <si>
-    <t>Pressure filter flitrate tank agitator exponent [0.4, 0.5, 0.6]</t>
-  </si>
-  <si>
-    <t>Pressure filter flitrate tank agitator electricity rate (kW / kg/hr) [0.000158, 0.000176, 0.000193]</t>
-  </si>
-  <si>
-    <t>Hydrolysate cooler heat exchanger base cost (USD) [7.65e+04, 8.5e+04, 9.35e+04]</t>
-  </si>
-  <si>
-    <t>Hydrolysate cooler heat exchanger exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Process water center tank base cost (USD) [2.25e+05, 2.5e+05, 2.75e+05]</t>
-  </si>
-  <si>
-    <t>Process water center tank exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Process water center process water pump base cost (USD) [1.38e+04, 1.53e+04, 1.68e+04]</t>
-  </si>
-  <si>
-    <t>Process water center process water pump exponent [0.7, 0.8, 0.9]</t>
-  </si>
-  <si>
-    <t>Process water center process water pump electricity rate (kW / kg/hr) [9.7e-05, 0.000108, 0.000119]</t>
-  </si>
-  <si>
-    <t>Process water center makeup water pump base cost (USD) [6.18e+03, 6.86e+03, 7.55e+03]</t>
-  </si>
-  <si>
-    <t>Process water center makeup water pump exponent [0.7, 0.8, 0.9]</t>
-  </si>
-  <si>
-    <t>Process water center makeup water pump electricity rate (kW / kg/hr) [8.63e-05, 9.59e-05, 0.000105]</t>
-  </si>
-  <si>
-    <t>Boiler turbogenerator boiler base cost (USD) [2.57e+07, 2.86e+07, 3.14e+07]</t>
-  </si>
-  <si>
-    <t>Boiler turbogenerator boiler exponent [0.5, 0.6, 0.7]</t>
-  </si>
-  <si>
-    <t>Boiler turbogenerator boiler electricity rate (kW / kg/hr) [0.00377, 0.00419, 0.00461]</t>
-  </si>
-  <si>
-    <t>Boiler turbogenerator deaerator base cost (USD) [2.74e+05, 3.05e+05, 3.36e+05]</t>
-  </si>
-  <si>
-    <t>Boiler turbogenerator deaerator exponent [0.5, 0.6, 0.7]</t>
-  </si>
-  <si>
-    <t>Boiler turbogenerator amine addition pkg base cost (USD) [3.6e+04, 4e+04, 4.4e+04]</t>
-  </si>
-  <si>
-    <t>Boiler turbogenerator amine addition pkg exponent [0.5, 0.6, 0.7]</t>
-  </si>
-  <si>
-    <t>Boiler turbogenerator hot process water softener system base cost (USD) [7.02e+04, 7.8e+04, 8.58e+04]</t>
-  </si>
-  <si>
-    <t>Boiler turbogenerator hot process water softener system exponent [0.5, 0.6, 0.7]</t>
-  </si>
-  <si>
-    <t>Boiler turbogenerator turbogenerator base cost (USD) [8.55e+06, 9.5e+06, 1.04e+07]</t>
-  </si>
-  <si>
-    <t>Boiler turbogenerator turbogenerator exponent [0.5, 0.6, 0.7]</t>
-  </si>
-  <si>
-    <t>Sulfuric acid tank tank base cost (USD) [5.59e+03, 6.21e+03, 6.83e+03]</t>
-  </si>
-  <si>
-    <t>Sulfuric acid tank tank exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Sulfuric acid tank pump base cost (USD) [7.2e+03, 8e+03, 8.8e+03]</t>
-  </si>
-  <si>
-    <t>Sulfuric acid tank pump exponent [0.7, 0.8, 0.9]</t>
-  </si>
-  <si>
-    <t>Sulfuric acid tank pump electricity rate (kW / kg/hr) [0.000242, 0.000269, 0.000296]</t>
-  </si>
-  <si>
-    <t>Enzyme hydrolysate mixer mixer base cost (USD) [9.81e+04, 1.09e+05, 1.2e+05]</t>
-  </si>
-  <si>
-    <t>Enzyme hydrolysate mixer mixer exponent [0.4, 0.5, 0.6]</t>
-  </si>
-  <si>
-    <t>Enzyme hydrolysate mixer mixer electricity rate (kW / kg/hr) [0.000177, 0.000196, 0.000216]</t>
+    <t>Beer tank tank base cost (USD) [5.72e+05, 6.36e+05, 7e+05]</t>
+  </si>
+  <si>
+    <t>Beer tank tank exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Beer tank pump base cost (USD) [2.41e+04, 2.68e+04, 2.95e+04]</t>
+  </si>
+  <si>
+    <t>Beer tank pump exponent [0.7, 0.8, 0.9]</t>
+  </si>
+  <si>
+    <t>Beer tank pump electricity rate (kW / kg/hr) [0.000197, 0.000219, 0.000241]</t>
+  </si>
+  <si>
+    <t>Beer tank agitator base cost (USD) [6.15e+04, 6.83e+04, 7.51e+04]</t>
+  </si>
+  <si>
+    <t>Beer tank agitator exponent [0.4, 0.5, 0.6]</t>
+  </si>
+  <si>
+    <t>Beer tank agitator electricity rate (kW / kg/hr) [3.15e-05, 3.5e-05, 3.85e-05]</t>
+  </si>
+  <si>
+    <t>Chilled water package base cost (USD) [1.24e+06, 1.38e+06, 1.51e+06]</t>
+  </si>
+  <si>
+    <t>Chilled water package exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Chilled water package electricity rate (kW / kJ/hr) [-3.9e-05, -4.33e-05, -4.76e-05]</t>
+  </si>
+  <si>
+    <t>CIP Package base cost (USD) [3.79e+05, 4.21e+05, 4.63e+05]</t>
+  </si>
+  <si>
+    <t>CIP Package exponent [0.5, 0.6, 0.7]</t>
+  </si>
+  <si>
+    <t>Cooling tower base cost (USD) [1.24e+06, 1.38e+06, 1.51e+06]</t>
+  </si>
+  <si>
+    <t>Cooling tower exponent [0.6, 0.7, 0.8]</t>
+  </si>
+  <si>
+    <t>Cooling tower electricity rate (kW / kmol/hr) [0.00258, 0.00287, 0.00315]</t>
+  </si>
+  <si>
+    <t>Cooling tower cooling water pump base cost (USD) [2.55e+05, 2.84e+05, 3.12e+05]</t>
+  </si>
+  <si>
+    <t>Cooling tower cooling water pump exponent [0.7, 0.8, 0.9]</t>
+  </si>
+  <si>
+    <t>Cooling tower cooling water pump electricity rate (kW / kmol/hr) [0.00165, 0.00183, 0.00202]</t>
   </si>
   <si>
     <t>Oligomer conversion tank tank base cost (USD) [1.83e+05, 2.03e+05, 2.23e+05]</t>
@@ -481,72 +577,6 @@
     <t>Oligomer conversion tank agitator electricity rate (kW / kg/hr) [0.000579, 0.000644, 0.000708]</t>
   </si>
   <si>
-    <t>Vent scrubber base cost (USD) [1.94e+05, 2.15e+05, 2.37e+05]</t>
-  </si>
-  <si>
-    <t>Vent scrubber exponent [0.5, 0.6, 0.7]</t>
-  </si>
-  <si>
-    <t>Pretreatment reactor system base cost (USD) [1.78e+07, 1.98e+07, 2.18e+07]</t>
-  </si>
-  <si>
-    <t>Pretreatment reactor system exponent [0.5, 0.6, 0.7]</t>
-  </si>
-  <si>
-    <t>Pretreatment reactor system electricity rate (kW / kg/hr) [0.0494, 0.0549, 0.0604]</t>
-  </si>
-  <si>
-    <t>Chilled water package base cost (USD) [1.24e+06, 1.38e+06, 1.51e+06]</t>
-  </si>
-  <si>
-    <t>Chilled water package exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Chilled water package electricity rate (kW / kJ/hr) [-3.9e-05, -4.33e-05, -4.76e-05]</t>
-  </si>
-  <si>
-    <t>Cooling tower base cost (USD) [1.24e+06, 1.38e+06, 1.51e+06]</t>
-  </si>
-  <si>
-    <t>Cooling tower exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Cooling tower electricity rate (kW / kmol/hr) [0.00258, 0.00287, 0.00315]</t>
-  </si>
-  <si>
-    <t>Cooling tower cooling water pump base cost (USD) [2.55e+05, 2.84e+05, 3.12e+05]</t>
-  </si>
-  <si>
-    <t>Cooling tower cooling water pump exponent [0.7, 0.8, 0.9]</t>
-  </si>
-  <si>
-    <t>Cooling tower cooling water pump electricity rate (kW / kmol/hr) [0.00165, 0.00183, 0.00202]</t>
-  </si>
-  <si>
-    <t>Beer tank tank base cost (USD) [5.72e+05, 6.36e+05, 7e+05]</t>
-  </si>
-  <si>
-    <t>Beer tank tank exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Beer tank pump base cost (USD) [2.41e+04, 2.68e+04, 2.95e+04]</t>
-  </si>
-  <si>
-    <t>Beer tank pump exponent [0.7, 0.8, 0.9]</t>
-  </si>
-  <si>
-    <t>Beer tank pump electricity rate (kW / kg/hr) [0.000197, 0.000219, 0.000241]</t>
-  </si>
-  <si>
-    <t>Beer tank agitator base cost (USD) [6.15e+04, 6.83e+04, 7.51e+04]</t>
-  </si>
-  <si>
-    <t>Beer tank agitator exponent [0.4, 0.5, 0.6]</t>
-  </si>
-  <si>
-    <t>Beer tank agitator electricity rate (kW / kg/hr) [3.15e-05, 3.5e-05, 3.85e-05]</t>
-  </si>
-  <si>
     <t>Blowdown discharge pump pump base cost (USD) [2.28e+04, 2.54e+04, 2.79e+04]</t>
   </si>
   <si>
@@ -601,51 +631,21 @@
     <t>Saccharification and co fermentation recirculation pumps electricity rate (kW / m3/hr) [0.35, 0.388, 0.427]</t>
   </si>
   <si>
-    <t>CIP Package base cost (USD) [3.79e+05, 4.21e+05, 4.63e+05]</t>
-  </si>
-  <si>
-    <t>CIP Package exponent [0.5, 0.6, 0.7]</t>
-  </si>
-  <si>
-    <t>Pretreatment flash tank base cost (USD) [4.6e+05, 5.11e+05, 5.62e+05]</t>
-  </si>
-  <si>
-    <t>Pretreatment flash tank exponent [0.6, 0.7, 0.8]</t>
-  </si>
-  <si>
-    <t>Pretreatment flash pump base cost (USD) [2.7e+04, 3e+04, 3.3e+04]</t>
-  </si>
-  <si>
-    <t>Pretreatment flash pump exponent [0.7, 0.8, 0.9]</t>
-  </si>
-  <si>
-    <t>Pretreatment flash pump electricity rate (kW / kg/hr) [0.000199, 0.000221, 0.000243]</t>
-  </si>
-  <si>
-    <t>Pretreatment flash agitator base cost (USD) [8.1e+04, 9e+04, 9.9e+04]</t>
-  </si>
-  <si>
-    <t>Pretreatment flash agitator exponent [0.4, 0.5, 0.6]</t>
-  </si>
-  <si>
-    <t>Pretreatment flash agitator electricity rate (kW / kg/hr) [0.000605, 0.000672, 0.000739]</t>
+    <t>Stream-makeup water price (USD/kg) [0.000228, 0.000254, 0.000279]</t>
+  </si>
+  <si>
+    <t>Stream-cellulase price (USD/kg) [0.191, 0.212, 0.233]</t>
+  </si>
+  <si>
+    <t>Stream-WWT caustic price (USD/kg) [0.0673, 0.0748, 0.0822]</t>
+  </si>
+  <si>
+    <t>Stream-Baghouse bags price (USD/kg) [9.99, 11.1, 12.2]</t>
   </si>
   <si>
     <t>Stream-ammonia price (USD/kg) [0.404, 0.449, 0.493]</t>
   </si>
   <si>
-    <t>Stream-makeup water price (USD/kg) [0.000228, 0.000254, 0.000279]</t>
-  </si>
-  <si>
-    <t>Stream-cellulase price (USD/kg) [0.191, 0.212, 0.233]</t>
-  </si>
-  <si>
-    <t>Stream-WWT caustic price (USD/kg) [0.0673, 0.0748, 0.0822]</t>
-  </si>
-  <si>
-    <t>Stream-Baghouse bags price (USD/kg) [9.99, 11.1, 12.2]</t>
-  </si>
-  <si>
     <t>Stream-cornstover price (USD/kg) [0.0464, 0.0516, 0.0567]</t>
   </si>
   <si>
@@ -661,10 +661,10 @@
     <t>Stream-sulfuric acid price (USD/kg) [0.0807, 0.0897, 0.0987]</t>
   </si>
   <si>
+    <t>Stream-ethanol price (USD/kg) [0.643, 0.715, 0.786]</t>
+  </si>
+  <si>
     <t>Stream-ash price (USD/kg) [-0.0286, -0.0318, -0.035]</t>
-  </si>
-  <si>
-    <t>Stream-ethanol price (USD/kg) [0.653, 0.726, 0.799]</t>
   </si>
   <si>
     <t>Electricity price (USD/kWhr) [0.0515, 0.0572, 0.0629]</t>
@@ -1065,7 +1065,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-0.5683048304830483</v>
+        <v>-0.5833063306330631</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1073,7 +1073,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-0.1908790879087909</v>
+        <v>-0.129000900090009</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1081,7 +1081,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-0.09294929492949294</v>
+        <v>-0.03885988598859886</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1089,7 +1089,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.06175817581758176</v>
+        <v>0.1831863186318632</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1097,7 +1097,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.01164116411641164</v>
+        <v>-0.1694449444944494</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1105,7 +1105,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-0.06681068106810681</v>
+        <v>-0.01780978097809781</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1113,7 +1113,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>-0.1596639663966396</v>
+        <v>-0.05689768976897689</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1121,7 +1121,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>-0.1383738373837383</v>
+        <v>0.116975697569757</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1129,7 +1129,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.03504350435043504</v>
+        <v>0.09406540654065405</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1137,7 +1137,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.03971197119711971</v>
+        <v>-0.04531653165316531</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1145,7 +1145,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>-0.02515451545154515</v>
+        <v>-0.1221242124212421</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1153,7 +1153,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.01195319531953195</v>
+        <v>-0.1147314731473147</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1161,7 +1161,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.01525352535253525</v>
+        <v>-0.0888088808880888</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1169,7 +1169,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.1233483348334833</v>
+        <v>0.1995799579957996</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1177,7 +1177,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>-0.02833483348334833</v>
+        <v>-0.1403180318031803</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1185,7 +1185,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.08919291929192917</v>
+        <v>-0.2113291329132913</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1193,7 +1193,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.007272727272727272</v>
+        <v>-0.05675367536753675</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1201,7 +1201,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.04729672967296729</v>
+        <v>0.03987998799879987</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1209,7 +1209,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.01788178817881788</v>
+        <v>-0.1263366336633663</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1217,7 +1217,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.02588658865886588</v>
+        <v>0.05074107410741074</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1225,7 +1225,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>-0.2143774377437744</v>
+        <v>0.01141314131413141</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1233,7 +1233,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>-0.1234323432343234</v>
+        <v>0.1531353135313531</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1241,7 +1241,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>0.1871347134713471</v>
+        <v>-0.1165316531653165</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1249,7 +1249,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>-0.1211641164116412</v>
+        <v>0.1982238223822382</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1257,7 +1257,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>-0.00726072607260726</v>
+        <v>0.04171617161716171</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1265,7 +1265,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>-0.1158835883588359</v>
+        <v>0.004524452445244524</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1273,7 +1273,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>-0.04622862286228623</v>
+        <v>0.141026102610261</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1281,7 +1281,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>-0.04162016201620161</v>
+        <v>0.02099009900990099</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1289,7 +1289,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>-0.01776177617761776</v>
+        <v>0.1608040804080408</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1297,7 +1297,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>-0.05963396339633963</v>
+        <v>-0.04159615961596159</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1305,7 +1305,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>-0.02695469546954695</v>
+        <v>-0.1996399639963996</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1313,7 +1313,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>-0.1405220522052205</v>
+        <v>0.03582358235823582</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1321,7 +1321,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>-0.0314071407140714</v>
+        <v>-0.009228922892289227</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1329,7 +1329,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>-0.0446084608460846</v>
+        <v>-0.115055505550555</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1337,7 +1337,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>0.1718931893189319</v>
+        <v>0.1198559855985598</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1345,7 +1345,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>0.009720972097209719</v>
+        <v>-0.09046504650465045</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1353,7 +1353,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>-0.06817881788178817</v>
+        <v>0.07134713471347134</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1361,7 +1361,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>-0.0036003600360036</v>
+        <v>-0.1363456345634563</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1369,7 +1369,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>0.09128112811281126</v>
+        <v>-0.00438043804380438</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1377,7 +1377,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>0.0422082208220822</v>
+        <v>-0.00048004800480048</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1385,7 +1385,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>0.01748574857485748</v>
+        <v>0.0008040804080408039</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1393,7 +1393,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>0.1644884488448844</v>
+        <v>0.1397659765976597</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1401,7 +1401,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>0.07888388838883888</v>
+        <v>-0.004428442844284428</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1409,7 +1409,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0.01938193819381938</v>
+        <v>0.1092229222922292</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1417,7 +1417,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>0.2111491149114911</v>
+        <v>-0.0291029102910291</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1425,7 +1425,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>-0.08003600360036003</v>
+        <v>0.1003180318031803</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1433,7 +1433,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>0.0432043204320432</v>
+        <v>0.08910891089108909</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1441,7 +1441,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>-0.0381998199819982</v>
+        <v>0.1843744374437443</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1449,7 +1449,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>0.00696069606960696</v>
+        <v>0.06583858385838583</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1457,7 +1457,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>0.01176117611761176</v>
+        <v>0.06832283228322832</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1465,7 +1465,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>-0.007584758475847584</v>
+        <v>0.01851785178517852</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1473,7 +1473,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>-0.1476747674767477</v>
+        <v>0.03531953195319532</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1481,7 +1481,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>-0.0342994299429943</v>
+        <v>-0.01983798379837984</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1489,7 +1489,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>-0.03114311431143114</v>
+        <v>-0.1726492649264926</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1497,7 +1497,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>-0.151995199519952</v>
+        <v>0.05622562256225622</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1505,7 +1505,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>0.09430543054305429</v>
+        <v>-0.07595559555955594</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1513,7 +1513,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>-0.1086468646864686</v>
+        <v>0.002352235223522352</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1521,7 +1521,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>-0.167992799279928</v>
+        <v>0.1963996399639964</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1529,7 +1529,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>-0.01218121812181218</v>
+        <v>0.0944134413441344</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1537,7 +1537,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>-0.00768076807680768</v>
+        <v>0.08208820882088208</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1545,7 +1545,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>-0.0366036603660366</v>
+        <v>-0.01528952895289529</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1553,7 +1553,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>-0.02144614461446144</v>
+        <v>-0.1191119111911191</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1561,7 +1561,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>-0.09023702370237023</v>
+        <v>0.03614761476147614</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1569,7 +1569,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>-0.05646564656465645</v>
+        <v>-0.09405340534053404</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1577,7 +1577,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>0.06355835583558356</v>
+        <v>0.1726132613261326</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1585,7 +1585,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>-0.0525052505250525</v>
+        <v>-0.2086528652865286</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1593,7 +1593,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>0.04326432643264326</v>
+        <v>-0.05048904890489049</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1601,7 +1601,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>-0.03368736873687368</v>
+        <v>0.002136213621362136</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1609,7 +1609,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>-0.0392079207920792</v>
+        <v>-0.1363816381638163</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1617,7 +1617,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>-0.1503990399039904</v>
+        <v>-0.02118211821182118</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1625,7 +1625,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>-0.1463066306630663</v>
+        <v>0.3221482148214821</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1633,7 +1633,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>-0.1807500750075007</v>
+        <v>0.05305730573057305</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1641,7 +1641,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>0.009036903690369035</v>
+        <v>-0.05767776777677767</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1649,7 +1649,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>-0.05808580858085808</v>
+        <v>0.03656765676567657</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1657,7 +1657,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>0.169096909690969</v>
+        <v>0.03653165316531653</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1665,7 +1665,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>0.07965196519651963</v>
+        <v>-0.03463546354635463</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1673,7 +1673,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>-0.1368136813681368</v>
+        <v>0.03642364236423642</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1681,7 +1681,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>-0.1338613861386138</v>
+        <v>0.04297629762976297</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1689,7 +1689,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>-0.1417221722172217</v>
+        <v>0.1258805880588059</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1697,7 +1697,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>0.1041824182418242</v>
+        <v>-0.03344734473447344</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1705,7 +1705,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>-0.04451245124512451</v>
+        <v>0.001212121212121212</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1713,7 +1713,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>0.01482148214821482</v>
+        <v>-0.0407080708070807</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1721,7 +1721,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>0.06335433543354334</v>
+        <v>-0.1711131113111311</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1729,7 +1729,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>0.1108430843084308</v>
+        <v>-0.0006480648064806481</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1737,7 +1737,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>-0.05449744974497449</v>
+        <v>0.02043804380438044</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1745,7 +1745,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>0.06923492349234923</v>
+        <v>0.08595259525952594</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1753,7 +1753,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>0.02571857185718571</v>
+        <v>-0.3041104110411041</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1761,7 +1761,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>0.03797179717971797</v>
+        <v>0.0387038703870387</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1769,7 +1769,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>-0.03404740474047404</v>
+        <v>0.1281848184818482</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1777,7 +1777,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>-0.2348394839483948</v>
+        <v>-0.02168616861686168</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1785,7 +1785,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>0.1667446744674467</v>
+        <v>-0.04556855685568556</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1793,7 +1793,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>0.02547854785478548</v>
+        <v>-0.2353675367536753</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1801,7 +1801,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>0.05926192619261925</v>
+        <v>0.04202820282028202</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1809,7 +1809,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>0.1073267326732673</v>
+        <v>-0.08556855685568555</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1817,7 +1817,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>-0.007020702070207019</v>
+        <v>0.08061206120612061</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1825,7 +1825,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>0.0458085808580858</v>
+        <v>-0.06636663666366636</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1833,7 +1833,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>-0.02784278427842784</v>
+        <v>0.08919291929192917</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1841,7 +1841,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>-0.1171917191719172</v>
+        <v>0.07858385838583858</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1849,7 +1849,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>-0.004200420042004199</v>
+        <v>0.09954995499549953</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1857,7 +1857,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>-0.05838583858385838</v>
+        <v>-0.08589258925892589</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1865,7 +1865,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>-0.02943894389438944</v>
+        <v>-0.09599759975997599</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1873,7 +1873,7 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>0.07573957395739574</v>
+        <v>-0.02695469546954695</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1881,7 +1881,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>-0.3181158115811581</v>
+        <v>0.09040504050405039</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1889,7 +1889,7 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>0.03528352835283528</v>
+        <v>0.00312031203120312</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1897,7 +1897,7 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>0.04012001200120011</v>
+        <v>0.02867086708670867</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1905,7 +1905,7 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>-0.1062106210621062</v>
+        <v>0.1398499849984998</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1913,7 +1913,7 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>0.1722892289228923</v>
+        <v>-0.04672067206720671</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1921,7 +1921,7 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>-0.02617461746174617</v>
+        <v>0.04742874287428742</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1929,7 +1929,7 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>0.1226402640264026</v>
+        <v>0.07557155715571556</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1937,7 +1937,7 @@
         <v>110</v>
       </c>
       <c r="B111">
-        <v>0.1476147614761476</v>
+        <v>0.05546954695469546</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1945,7 +1945,7 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>0.00564056405640564</v>
+        <v>0.02771077107710771</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1953,7 +1953,7 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>-0.0390999099909991</v>
+        <v>-0.09225322532253223</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1961,7 +1961,7 @@
         <v>113</v>
       </c>
       <c r="B114">
-        <v>-0.01186918691869187</v>
+        <v>-0.1954755475547555</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1969,7 +1969,7 @@
         <v>114</v>
       </c>
       <c r="B115">
-        <v>0.1323492349234923</v>
+        <v>0.06459045904590459</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1977,7 +1977,7 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>-0.02232223222322232</v>
+        <v>0.02155415541554155</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1985,7 +1985,7 @@
         <v>116</v>
       </c>
       <c r="B117">
-        <v>0.01466546654665466</v>
+        <v>-0.1581758175817581</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1993,7 +1993,7 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>-0.07147914791479147</v>
+        <v>-0.2396639663966396</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2001,7 +2001,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>-0.09208520852085207</v>
+        <v>0.09664566456645664</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2009,7 +2009,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>-0.06390639063906389</v>
+        <v>-0.02083408340834083</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2017,7 +2017,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>-0.06845484548454844</v>
+        <v>0.02567056705670567</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2025,7 +2025,7 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>-0.1545634563456345</v>
+        <v>-0.0496129612961296</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2033,7 +2033,7 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>0.06837083708370838</v>
+        <v>0.05101710171017101</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2041,7 +2041,7 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>0.1775097509750975</v>
+        <v>-0.004404440444044404</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2049,7 +2049,7 @@
         <v>124</v>
       </c>
       <c r="B125">
-        <v>-0.06335433543354334</v>
+        <v>0.05239723972397239</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2057,7 +2057,7 @@
         <v>125</v>
       </c>
       <c r="B126">
-        <v>0.01256525652565256</v>
+        <v>0.01881788178817882</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2065,7 +2065,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>-0.1808460846084608</v>
+        <v>-0.0869246924692469</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2073,7 +2073,7 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>-0.03647164716471647</v>
+        <v>-0.05465346534653465</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2081,7 +2081,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>0.05922592259225921</v>
+        <v>0.008784878487848783</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2089,7 +2089,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>0.04332433243324332</v>
+        <v>0.1747854785478548</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2097,7 +2097,7 @@
         <v>130</v>
       </c>
       <c r="B131">
-        <v>0.03035103510351034</v>
+        <v>-0.1081068106810681</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2105,7 +2105,7 @@
         <v>131</v>
       </c>
       <c r="B132">
-        <v>0.03409540954095409</v>
+        <v>0.01785778577857786</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -2113,7 +2113,7 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>-0.04262826282628263</v>
+        <v>-0.08136813681368135</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2121,7 +2121,7 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>-0.1349414941494149</v>
+        <v>-0.2138853885388539</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2129,7 +2129,7 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>-0.07528352835283528</v>
+        <v>-0.02017401740174017</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2137,7 +2137,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>0.08682868286828681</v>
+        <v>-0.05053705370537052</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2145,7 +2145,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>0.03965196519651965</v>
+        <v>-0.01474947494749475</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2153,7 +2153,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>0.05136513651365136</v>
+        <v>-0.02645064506450645</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2161,7 +2161,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>0.001044104410441044</v>
+        <v>-0.1914431443144314</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2169,7 +2169,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>-0.04255625562556255</v>
+        <v>0.1713891389138914</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2177,7 +2177,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>-0.002028202820282028</v>
+        <v>0.1464026402640264</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2185,7 +2185,7 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>0.04661266126612661</v>
+        <v>0.01144914491449145</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2193,7 +2193,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>-0.06117011701170116</v>
+        <v>0.06585058505850584</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2201,7 +2201,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>0.05615361536153615</v>
+        <v>0.01425742574257426</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2209,7 +2209,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>0.02767476747674767</v>
+        <v>-0.1013861386138614</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2217,7 +2217,7 @@
         <v>145</v>
       </c>
       <c r="B146">
-        <v>-0.1651965196519652</v>
+        <v>0.00312031203120312</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2225,7 +2225,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>0.007452745274527452</v>
+        <v>0.09297329732973296</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2233,7 +2233,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>0.04172817281728172</v>
+        <v>-0.04324032403240324</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2241,7 +2241,7 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>0.1092949294929493</v>
+        <v>0.1353135313531353</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2249,7 +2249,7 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>-0.267038703870387</v>
+        <v>0.007776777677767775</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2257,7 +2257,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>-0.1202760276027603</v>
+        <v>-0.2264386438643864</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2265,7 +2265,7 @@
         <v>151</v>
       </c>
       <c r="B152">
-        <v>-0.061002100210021</v>
+        <v>-0.005088508850885087</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -2273,7 +2273,7 @@
         <v>152</v>
       </c>
       <c r="B153">
-        <v>0.1052745274527453</v>
+        <v>-0.1888388838883888</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2281,7 +2281,7 @@
         <v>153</v>
       </c>
       <c r="B154">
-        <v>-0.1536513651365136</v>
+        <v>-0.09652565256525653</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -2289,7 +2289,7 @@
         <v>154</v>
       </c>
       <c r="B155">
-        <v>-0.08224422442244222</v>
+        <v>0.02469846984698469</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -2297,7 +2297,7 @@
         <v>155</v>
       </c>
       <c r="B156">
-        <v>0.1005340534053405</v>
+        <v>0.01096909690969097</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -2305,7 +2305,7 @@
         <v>156</v>
       </c>
       <c r="B157">
-        <v>0.005376537653765376</v>
+        <v>-0.05845784578457845</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -2313,7 +2313,7 @@
         <v>157</v>
       </c>
       <c r="B158">
-        <v>0.1076147614761476</v>
+        <v>0.08685268526852684</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -2321,7 +2321,7 @@
         <v>158</v>
       </c>
       <c r="B159">
-        <v>-0.2340834083408341</v>
+        <v>0.1867866786678668</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -2329,7 +2329,7 @@
         <v>159</v>
       </c>
       <c r="B160">
-        <v>-0.1418421842184218</v>
+        <v>-0.04661266126612661</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -2337,7 +2337,7 @@
         <v>160</v>
       </c>
       <c r="B161">
-        <v>0.04296429642964296</v>
+        <v>-0.1103150315031503</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -2345,7 +2345,7 @@
         <v>161</v>
       </c>
       <c r="B162">
-        <v>0.02384638463846384</v>
+        <v>-0.07248724872487249</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -2353,7 +2353,7 @@
         <v>162</v>
       </c>
       <c r="B163">
-        <v>-0.1597359735973597</v>
+        <v>-0.1711251125112511</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -2361,7 +2361,7 @@
         <v>163</v>
       </c>
       <c r="B164">
-        <v>0.1146474647464746</v>
+        <v>-0.08338433843384338</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -2369,7 +2369,7 @@
         <v>164</v>
       </c>
       <c r="B165">
-        <v>0.03219921992199219</v>
+        <v>0.1378577857785779</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -2377,7 +2377,7 @@
         <v>165</v>
       </c>
       <c r="B166">
-        <v>-0.1186198619861986</v>
+        <v>-0.1134833483348335</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -2385,7 +2385,7 @@
         <v>166</v>
       </c>
       <c r="B167">
-        <v>0.1095589558955895</v>
+        <v>-0.02438643864386438</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -2393,7 +2393,7 @@
         <v>167</v>
       </c>
       <c r="B168">
-        <v>0.06277827782778277</v>
+        <v>-0.158991899189919</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -2401,7 +2401,7 @@
         <v>168</v>
       </c>
       <c r="B169">
-        <v>0.121056105610561</v>
+        <v>0.03753975397539754</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -2409,7 +2409,7 @@
         <v>169</v>
       </c>
       <c r="B170">
-        <v>0.1006420642064206</v>
+        <v>0.03203120312031203</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -2417,7 +2417,7 @@
         <v>170</v>
       </c>
       <c r="B171">
-        <v>-0.1233363336333633</v>
+        <v>0.008736873687368736</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -2425,7 +2425,7 @@
         <v>171</v>
       </c>
       <c r="B172">
-        <v>0.159027902790279</v>
+        <v>0.07812781278127812</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -2433,7 +2433,7 @@
         <v>172</v>
       </c>
       <c r="B173">
-        <v>-0.1333213321332133</v>
+        <v>-0.009084908490849083</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2441,7 +2441,7 @@
         <v>173</v>
       </c>
       <c r="B174">
-        <v>0.06444644464446445</v>
+        <v>-0.106990699069907</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -2449,7 +2449,7 @@
         <v>174</v>
       </c>
       <c r="B175">
-        <v>-0.1639003900390039</v>
+        <v>-0.01436543654365436</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2457,7 +2457,7 @@
         <v>175</v>
       </c>
       <c r="B176">
-        <v>-0.1075067506750675</v>
+        <v>-0.181014101410141</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -2465,7 +2465,7 @@
         <v>176</v>
       </c>
       <c r="B177">
-        <v>-0.1226642664266426</v>
+        <v>-0.01299729972997299</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -2473,7 +2473,7 @@
         <v>177</v>
       </c>
       <c r="B178">
-        <v>-0.02436243624362436</v>
+        <v>-0.02243024302430243</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -2481,7 +2481,7 @@
         <v>178</v>
       </c>
       <c r="B179">
-        <v>0.2114251425142514</v>
+        <v>0.03522352235223522</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -2489,7 +2489,7 @@
         <v>179</v>
       </c>
       <c r="B180">
-        <v>0.004092409240924091</v>
+        <v>-0.0857125712571257</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -2497,7 +2497,7 @@
         <v>180</v>
       </c>
       <c r="B181">
-        <v>0.06277827782778277</v>
+        <v>0.01195319531953195</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -2505,7 +2505,7 @@
         <v>181</v>
       </c>
       <c r="B182">
-        <v>0.04152415241524152</v>
+        <v>0.1046264626462646</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -2513,7 +2513,7 @@
         <v>182</v>
       </c>
       <c r="B183">
-        <v>-0.09803780378037803</v>
+        <v>-0.01964596459645964</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -2521,7 +2521,7 @@
         <v>183</v>
       </c>
       <c r="B184">
-        <v>-0.0431083108310831</v>
+        <v>-0.08680468046804679</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -2529,7 +2529,7 @@
         <v>184</v>
       </c>
       <c r="B185">
-        <v>-0.05638163816381637</v>
+        <v>0.09765376537653764</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -2537,7 +2537,7 @@
         <v>185</v>
       </c>
       <c r="B186">
-        <v>0.035007500750075</v>
+        <v>-0.06046204620462046</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -2545,7 +2545,7 @@
         <v>186</v>
       </c>
       <c r="B187">
-        <v>-0.07722772277227721</v>
+        <v>-0.05045304530453045</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -2553,7 +2553,7 @@
         <v>187</v>
       </c>
       <c r="B188">
-        <v>0.05645364536453645</v>
+        <v>0.1502550255025502</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -2561,7 +2561,7 @@
         <v>188</v>
       </c>
       <c r="B189">
-        <v>-0.09756975697569756</v>
+        <v>-0.06419441944194419</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -2569,7 +2569,7 @@
         <v>189</v>
       </c>
       <c r="B190">
-        <v>-0.08736873687368735</v>
+        <v>-0.06905490549054905</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -2577,7 +2577,7 @@
         <v>190</v>
       </c>
       <c r="B191">
-        <v>0.06456645664566456</v>
+        <v>-0.01729372937293729</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -2585,7 +2585,7 @@
         <v>191</v>
       </c>
       <c r="B192">
-        <v>0.1374137413741374</v>
+        <v>-0.1711371137113711</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -2593,7 +2593,7 @@
         <v>192</v>
       </c>
       <c r="B193">
-        <v>-0.02649864986498649</v>
+        <v>0.05557755775577557</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -2601,7 +2601,7 @@
         <v>193</v>
       </c>
       <c r="B194">
-        <v>0.1246684668466846</v>
+        <v>0.1002820282028203</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -2609,7 +2609,7 @@
         <v>194</v>
       </c>
       <c r="B195">
-        <v>-0.01596159615961596</v>
+        <v>-0.002376237623762376</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -2617,7 +2617,7 @@
         <v>195</v>
       </c>
       <c r="B196">
-        <v>-0.05594959495949594</v>
+        <v>0.08015601560156013</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -2625,7 +2625,7 @@
         <v>196</v>
       </c>
       <c r="B197">
-        <v>0.05365736573657365</v>
+        <v>-0.05764176417641764</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -2633,7 +2633,7 @@
         <v>197</v>
       </c>
       <c r="B198">
-        <v>0.002724272427242724</v>
+        <v>-0.04967296729672967</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -2641,7 +2641,7 @@
         <v>198</v>
       </c>
       <c r="B199">
-        <v>0.1071947194719472</v>
+        <v>0.04396039603960395</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -2649,7 +2649,7 @@
         <v>199</v>
       </c>
       <c r="B200">
-        <v>-0.1338493849384938</v>
+        <v>0.001308130813081308</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -2657,7 +2657,7 @@
         <v>200</v>
       </c>
       <c r="B201">
-        <v>-0.00636063606360636</v>
+        <v>0.05368136813681367</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -2665,7 +2665,7 @@
         <v>201</v>
       </c>
       <c r="B202">
-        <v>-0.0770957095709571</v>
+        <v>-0.0107050705070507</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -2673,7 +2673,7 @@
         <v>202</v>
       </c>
       <c r="B203">
-        <v>0.1404140414041404</v>
+        <v>0.05926192619261925</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -2681,7 +2681,7 @@
         <v>203</v>
       </c>
       <c r="B204">
-        <v>-0.001896189618961896</v>
+        <v>-0.1035343534353435</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -2689,7 +2689,7 @@
         <v>204</v>
       </c>
       <c r="B205">
-        <v>-0.02678667866786678</v>
+        <v>0.181014101410141</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -2697,7 +2697,7 @@
         <v>205</v>
       </c>
       <c r="B206">
-        <v>0.0596099609960996</v>
+        <v>0.08738073807380738</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -2705,7 +2705,7 @@
         <v>206</v>
       </c>
       <c r="B207">
-        <v>0.09648964896489648</v>
+        <v>0.3505070507050704</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -2713,7 +2713,7 @@
         <v>207</v>
       </c>
       <c r="B208">
-        <v>0.1691809180918092</v>
+        <v>-0.07036303630363036</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -2721,7 +2721,7 @@
         <v>208</v>
       </c>
       <c r="B209">
-        <v>-0.08277227722772276</v>
+        <v>-0.06131413141314131</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -2729,7 +2729,7 @@
         <v>209</v>
       </c>
       <c r="B210">
-        <v>-0.004956495649564956</v>
+        <v>-0.009588958895889586</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2737,7 +2737,7 @@
         <v>210</v>
       </c>
       <c r="B211">
-        <v>0.3604560456045603</v>
+        <v>0.5536153615361535</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -2745,7 +2745,7 @@
         <v>211</v>
       </c>
       <c r="B212">
-        <v>0.03727572757275727</v>
+        <v>0.3274167416741674</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -2753,7 +2753,7 @@
         <v>212</v>
       </c>
       <c r="B213">
-        <v>0.07429942994299429</v>
+        <v>0.2023642364236423</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -2761,7 +2761,7 @@
         <v>213</v>
       </c>
       <c r="B214">
-        <v>0.01392139213921392</v>
+        <v>-0.1187518751875187</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -2769,7 +2769,7 @@
         <v>214</v>
       </c>
       <c r="B215">
-        <v>-0.06820282028202819</v>
+        <v>0.04876087608760876</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -2777,7 +2777,7 @@
         <v>215</v>
       </c>
       <c r="B216">
-        <v>-0.00276027602760276</v>
+        <v>0.06545454545454545</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -2785,7 +2785,7 @@
         <v>216</v>
       </c>
       <c r="B217">
-        <v>0.02708670867086708</v>
+        <v>0.1323732373237324</v>
       </c>
     </row>
     <row r="218" spans="1:2">
@@ -2793,7 +2793,7 @@
         <v>217</v>
       </c>
       <c r="B218">
-        <v>-0.2607500750075007</v>
+        <v>-0.0378037803780378</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -2801,7 +2801,7 @@
         <v>218</v>
       </c>
       <c r="B219">
-        <v>0.04368436843684367</v>
+        <v>-0.02754275427542754</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -2809,7 +2809,7 @@
         <v>219</v>
       </c>
       <c r="B220">
-        <v>0.0859165916591659</v>
+        <v>-0.07062706270627062</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -2817,7 +2817,7 @@
         <v>220</v>
       </c>
       <c r="B221">
-        <v>0.1413861386138614</v>
+        <v>0.05154515451545154</v>
       </c>
     </row>
     <row r="222" spans="1:2">
@@ -2825,7 +2825,7 @@
         <v>221</v>
       </c>
       <c r="B222">
-        <v>0.03843984398439844</v>
+        <v>-0.0267026702670267</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -2833,7 +2833,7 @@
         <v>222</v>
       </c>
       <c r="B223">
-        <v>0.2146294629462946</v>
+        <v>0.2432883288328833</v>
       </c>
     </row>
     <row r="224" spans="1:2">
@@ -2841,7 +2841,7 @@
         <v>223</v>
       </c>
       <c r="B224">
-        <v>0.1004980498049805</v>
+        <v>-0.02129012901290129</v>
       </c>
     </row>
     <row r="225" spans="1:2">
@@ -2849,7 +2849,7 @@
         <v>224</v>
       </c>
       <c r="B225">
-        <v>-0.001968196819681968</v>
+        <v>-0.07714371437143713</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -2857,7 +2857,7 @@
         <v>225</v>
       </c>
       <c r="B226">
-        <v>0.1459105910591059</v>
+        <v>-0.04813681368136813</v>
       </c>
     </row>
   </sheetData>

</xml_diff>